<commit_message>
Decided to add a test case
</commit_message>
<xml_diff>
--- a/ConsecutiveOnes.xlsx
+++ b/ConsecutiveOnes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AEE73CD8-E5A4-4AD0-BE35-64F5E1D3A9DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB69C9AA-D1F7-4CE2-A6DD-F8A55DAAD566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{6D3CB909-E88B-4088-A601-EBBEB956DEC5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6D3CB909-E88B-4088-A601-EBBEB956DEC5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>String</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=I5R5WUDI_zI</t>
+  </si>
+  <si>
+    <t>1,1,0,0,0,0,0,0,1,1,1,1</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A369E89-EA67-45DE-9802-A7834BF0E19A}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -471,7 +474,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="str" cm="1">
-        <f t="array" ref="B3:B10">_xlfn.MAP(A3:A10,_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.a,LEN(SUBSTITUTE(_xlfn.TEXTSPLIT(_xlpm.x,0),",","")),_xlfn.TEXTJOIN(",",1,IF(_xlpm.a&gt;1,_xlpm.a,"")))))</f>
+        <f t="array" ref="B3:B11">_xlfn.MAP(A3:A11,_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.a,LEN(SUBSTITUTE(_xlfn.TEXTSPLIT(_xlpm.x,0),",","")),_xlfn.TEXTJOIN(",",1,IF(_xlpm.a&gt;1,_xlpm.a,"")))))</f>
         <v>2</v>
       </c>
     </row>
@@ -529,6 +532,14 @@
       </c>
       <c r="B10" t="str">
         <v>2,2,2,2,2,2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="str">
+        <v>2,4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>